<commit_message>
Acabados la monitorizacion de la CPU y RAM
</commit_message>
<xml_diff>
--- a/MonitorizacionCPU.xlsx
+++ b/MonitorizacionCPU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignasi\Downloads\DocumentosUIB\2n - 2n - ACSI\Practica Tema 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D6A7BC-15AA-40A2-81FC-148DE6A481F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37D0BD6-5650-4BAD-BA11-B92CB914C354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="1090">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="1089">
   <si>
     <t>Timestamp</t>
   </si>
@@ -3338,9 +3338,6 @@
       </rPr>
       <t xml:space="preserve"> ,que quiere decir que nuestro sistema cuenta con 16 CPUs.</t>
     </r>
-  </si>
-  <si>
-    <t>Monitorizando el uso de CPU del monitor TOP hemos obtenido los mismos 3 valores, por tanto, hemos contabilizado la frecuencia de cada uno de ellos. Valor: 0.0 - Frecuencia: 410, Valor: 0.2 - Frecuencia: 612, Valor: 0.4 - Frecuencia: 58. Que hacen una media de porcentaje de uso de CPU de: 0.13481398</t>
   </si>
 </sst>
 </file>
@@ -24249,8 +24246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1081"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24353,8 +24350,9 @@
       <c r="F5" t="s">
         <v>1087</v>
       </c>
-      <c r="G5" t="s">
-        <v>1089</v>
+      <c r="G5" t="str">
+        <f xml:space="preserve"> "La sobrecarga equivale a tiempo de ejecución del monitor entre el intervalo de medida = "&amp;(0.175/5)*100&amp;"%"</f>
+        <v>La sobrecarga equivale a tiempo de ejecución del monitor entre el intervalo de medida = 3,5%</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Acabados retoques finales, falta hacer el pdf
</commit_message>
<xml_diff>
--- a/MonitorizacionCPU.xlsx
+++ b/MonitorizacionCPU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignasi\Downloads\DocumentosUIB\2n - 2n - ACSI\Practica Tema 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37D0BD6-5650-4BAD-BA11-B92CB914C354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0D7796-1685-499C-8524-B20D6ACEA82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23921,13 +23921,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>609598</xdr:colOff>
+      <xdr:colOff>609599</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>10048875</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>9526</xdr:rowOff>
     </xdr:to>
@@ -24246,8 +24246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1081"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="G2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39422,6 +39422,7 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>